<commit_message>
Update Teknoloji Hazırlık Seviye Belirleme.xlsx
</commit_message>
<xml_diff>
--- a/Hafta 7/Teknolojik Hazırlık Seviyesi/Teknoloji Hazırlık Seviye Belirleme.xlsx
+++ b/Hafta 7/Teknolojik Hazırlık Seviyesi/Teknoloji Hazırlık Seviye Belirleme.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="CeuZm2jxRJpAhm+6dJEDRCYXoius3MVyfRLlyxTpRGw097RcHuDQMSIGCg3HNeb3duipRuFStui5jq/R2UFCAg==" workbookSaltValue="4yTIFfRXvesdrWQCtecOCA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" tabRatio="794" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17940" windowHeight="5844" tabRatio="794" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Genel-Mühendislik-Sistem" sheetId="6" r:id="rId1"/>
@@ -3531,29 +3531,9 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3579,19 +3559,37 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3606,6 +3604,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3614,6 +3618,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3641,16 +3651,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4281,7 +4281,7 @@
   </sheetPr>
   <dimension ref="A1:AU769"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -4297,15 +4297,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" s="1" customFormat="1" ht="372.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="77"/>
-      <c r="B1" s="78"/>
-      <c r="C1" s="79" t="s">
+      <c r="A1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="90" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
       <c r="H1" s="32" t="s">
         <v>136</v>
       </c>
@@ -4347,19 +4347,19 @@
       <c r="AO1" s="3"/>
     </row>
     <row r="2" spans="1:47" ht="101.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="92"/>
+      <c r="C2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="91" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="84" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4384,7 +4384,7 @@
       <c r="H3" s="12">
         <v>5</v>
       </c>
-      <c r="I3" s="92"/>
+      <c r="I3" s="85"/>
     </row>
     <row r="4" spans="1:47" s="9" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
@@ -4472,7 +4472,7 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="80">
+      <c r="A6" s="86">
         <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -4482,7 +4482,7 @@
       <c r="D6" s="52"/>
       <c r="E6" s="74"/>
       <c r="F6" s="52"/>
-      <c r="G6" s="116" t="s">
+      <c r="G6" s="77" t="s">
         <v>345</v>
       </c>
       <c r="H6" s="74"/>
@@ -4492,7 +4492,7 @@
       </c>
     </row>
     <row r="7" spans="1:47" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="80"/>
+      <c r="A7" s="86"/>
       <c r="B7" s="11" t="s">
         <v>145</v>
       </c>
@@ -4500,7 +4500,7 @@
       <c r="D7" s="52"/>
       <c r="E7" s="74"/>
       <c r="F7" s="52"/>
-      <c r="G7" s="116" t="s">
+      <c r="G7" s="77" t="s">
         <v>345</v>
       </c>
       <c r="H7" s="76"/>
@@ -4510,7 +4510,7 @@
       </c>
     </row>
     <row r="8" spans="1:47" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="80"/>
+      <c r="A8" s="86"/>
       <c r="B8" s="11" t="s">
         <v>146</v>
       </c>
@@ -4526,7 +4526,7 @@
       </c>
     </row>
     <row r="9" spans="1:47" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="80"/>
+      <c r="A9" s="86"/>
       <c r="B9" s="11" t="s">
         <v>147</v>
       </c>
@@ -4542,7 +4542,7 @@
       </c>
     </row>
     <row r="10" spans="1:47" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="80"/>
+      <c r="A10" s="86"/>
       <c r="B10" s="11" t="s">
         <v>148</v>
       </c>
@@ -4576,7 +4576,7 @@
       </c>
     </row>
     <row r="12" spans="1:47" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="80">
+      <c r="A12" s="86">
         <v>2</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -4594,7 +4594,7 @@
       </c>
     </row>
     <row r="13" spans="1:47" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="80"/>
+      <c r="A13" s="86"/>
       <c r="B13" s="11" t="s">
         <v>151</v>
       </c>
@@ -4610,7 +4610,7 @@
       </c>
     </row>
     <row r="14" spans="1:47" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="80"/>
+      <c r="A14" s="86"/>
       <c r="B14" s="11" t="s">
         <v>152</v>
       </c>
@@ -4626,7 +4626,7 @@
       </c>
     </row>
     <row r="15" spans="1:47" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="80"/>
+      <c r="A15" s="86"/>
       <c r="B15" s="11" t="s">
         <v>153</v>
       </c>
@@ -4642,7 +4642,7 @@
       </c>
     </row>
     <row r="16" spans="1:47" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="80"/>
+      <c r="A16" s="86"/>
       <c r="B16" s="11" t="s">
         <v>154</v>
       </c>
@@ -4676,7 +4676,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="80">
+      <c r="A18" s="86">
         <v>3</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -4694,7 +4694,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="80"/>
+      <c r="A19" s="86"/>
       <c r="B19" s="11" t="s">
         <v>157</v>
       </c>
@@ -4710,7 +4710,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="80"/>
+      <c r="A20" s="86"/>
       <c r="B20" s="11" t="s">
         <v>158</v>
       </c>
@@ -4726,7 +4726,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="80"/>
+      <c r="A21" s="86"/>
       <c r="B21" s="11" t="s">
         <v>159</v>
       </c>
@@ -4742,7 +4742,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="80"/>
+      <c r="A22" s="86"/>
       <c r="B22" s="11" t="s">
         <v>160</v>
       </c>
@@ -4758,7 +4758,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" s="37" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="80"/>
+      <c r="A23" s="86"/>
       <c r="B23" s="11" t="s">
         <v>161</v>
       </c>
@@ -4774,7 +4774,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="80"/>
+      <c r="A24" s="86"/>
       <c r="B24" s="11" t="s">
         <v>162</v>
       </c>
@@ -4808,7 +4808,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="80">
+      <c r="A26" s="86">
         <v>4</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -4826,7 +4826,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="80"/>
+      <c r="A27" s="86"/>
       <c r="B27" s="11" t="s">
         <v>165</v>
       </c>
@@ -4842,7 +4842,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" s="37" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="80"/>
+      <c r="A28" s="86"/>
       <c r="B28" s="11" t="s">
         <v>166</v>
       </c>
@@ -4858,7 +4858,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" s="37" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="80"/>
+      <c r="A29" s="86"/>
       <c r="B29" s="11" t="s">
         <v>167</v>
       </c>
@@ -4874,7 +4874,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="80"/>
+      <c r="A30" s="86"/>
       <c r="B30" s="11" t="s">
         <v>168</v>
       </c>
@@ -4890,7 +4890,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" s="37" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="80"/>
+      <c r="A31" s="86"/>
       <c r="B31" s="11" t="s">
         <v>169</v>
       </c>
@@ -4924,7 +4924,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="80">
+      <c r="A33" s="86">
         <v>5</v>
       </c>
       <c r="B33" s="11" t="s">
@@ -4942,7 +4942,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="80"/>
+      <c r="A34" s="86"/>
       <c r="B34" s="11" t="s">
         <v>172</v>
       </c>
@@ -4958,7 +4958,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" s="37" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="80"/>
+      <c r="A35" s="86"/>
       <c r="B35" s="11" t="s">
         <v>173</v>
       </c>
@@ -4974,7 +4974,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="80"/>
+      <c r="A36" s="86"/>
       <c r="B36" s="11" t="s">
         <v>174</v>
       </c>
@@ -4990,7 +4990,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="80"/>
+      <c r="A37" s="86"/>
       <c r="B37" s="11" t="s">
         <v>175</v>
       </c>
@@ -5024,7 +5024,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" s="37" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="80">
+      <c r="A39" s="86">
         <v>6</v>
       </c>
       <c r="B39" s="11" t="s">
@@ -5042,7 +5042,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="80"/>
+      <c r="A40" s="86"/>
       <c r="B40" s="11" t="s">
         <v>178</v>
       </c>
@@ -5058,7 +5058,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="80"/>
+      <c r="A41" s="86"/>
       <c r="B41" s="11" t="s">
         <v>179</v>
       </c>
@@ -5074,7 +5074,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="80"/>
+      <c r="A42" s="86"/>
       <c r="B42" s="11" t="s">
         <v>180</v>
       </c>
@@ -5090,7 +5090,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="80"/>
+      <c r="A43" s="86"/>
       <c r="B43" s="11" t="s">
         <v>181</v>
       </c>
@@ -5124,7 +5124,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="80">
+      <c r="A45" s="86">
         <v>7</v>
       </c>
       <c r="B45" s="11" t="s">
@@ -5142,7 +5142,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="80"/>
+      <c r="A46" s="86"/>
       <c r="B46" s="11" t="s">
         <v>184</v>
       </c>
@@ -5158,7 +5158,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="80"/>
+      <c r="A47" s="86"/>
       <c r="B47" s="11" t="s">
         <v>185</v>
       </c>
@@ -5174,7 +5174,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="80"/>
+      <c r="A48" s="86"/>
       <c r="B48" s="11" t="s">
         <v>186</v>
       </c>
@@ -5208,7 +5208,7 @@
       </c>
     </row>
     <row r="50" spans="1:47" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="80">
+      <c r="A50" s="86">
         <v>8</v>
       </c>
       <c r="B50" s="11" t="s">
@@ -5226,7 +5226,7 @@
       </c>
     </row>
     <row r="51" spans="1:47" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="80"/>
+      <c r="A51" s="86"/>
       <c r="B51" s="11" t="s">
         <v>189</v>
       </c>
@@ -5242,7 +5242,7 @@
       </c>
     </row>
     <row r="52" spans="1:47" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="80"/>
+      <c r="A52" s="86"/>
       <c r="B52" s="11" t="s">
         <v>190</v>
       </c>
@@ -5314,7 +5314,7 @@
       <c r="AU53" s="37"/>
     </row>
     <row r="54" spans="1:47" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="80">
+      <c r="A54" s="86">
         <v>9</v>
       </c>
       <c r="B54" s="11" t="s">
@@ -5332,7 +5332,7 @@
       </c>
     </row>
     <row r="55" spans="1:47" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="80"/>
+      <c r="A55" s="86"/>
       <c r="B55" s="39" t="s">
         <v>194</v>
       </c>
@@ -5348,7 +5348,7 @@
       </c>
     </row>
     <row r="56" spans="1:47" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="80"/>
+      <c r="A56" s="86"/>
       <c r="B56" s="11" t="s">
         <v>195</v>
       </c>
@@ -5364,7 +5364,7 @@
       </c>
     </row>
     <row r="57" spans="1:47" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="80"/>
+      <c r="A57" s="86"/>
       <c r="B57" s="11" t="s">
         <v>196</v>
       </c>
@@ -5380,36 +5380,36 @@
       </c>
     </row>
     <row r="58" spans="1:47" s="37" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="93"/>
-      <c r="B58" s="93"/>
+      <c r="A58" s="87"/>
+      <c r="B58" s="87"/>
       <c r="C58" s="40"/>
       <c r="D58" s="40"/>
       <c r="E58" s="40"/>
       <c r="F58" s="40"/>
     </row>
     <row r="59" spans="1:47" s="37" customFormat="1" ht="172.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="85" t="s">
+      <c r="A59" s="78" t="s">
         <v>197</v>
       </c>
-      <c r="B59" s="86"/>
-      <c r="C59" s="86"/>
-      <c r="D59" s="86"/>
-      <c r="E59" s="86"/>
-      <c r="F59" s="86"/>
-      <c r="G59" s="86"/>
-      <c r="H59" s="86"/>
-      <c r="I59" s="87"/>
+      <c r="B59" s="79"/>
+      <c r="C59" s="79"/>
+      <c r="D59" s="79"/>
+      <c r="E59" s="79"/>
+      <c r="F59" s="79"/>
+      <c r="G59" s="79"/>
+      <c r="H59" s="79"/>
+      <c r="I59" s="80"/>
     </row>
     <row r="60" spans="1:47" s="37" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="88"/>
-      <c r="B60" s="89"/>
-      <c r="C60" s="89"/>
-      <c r="D60" s="89"/>
-      <c r="E60" s="89"/>
-      <c r="F60" s="89"/>
-      <c r="G60" s="89"/>
-      <c r="H60" s="89"/>
-      <c r="I60" s="90"/>
+      <c r="A60" s="81"/>
+      <c r="B60" s="82"/>
+      <c r="C60" s="82"/>
+      <c r="D60" s="82"/>
+      <c r="E60" s="82"/>
+      <c r="F60" s="82"/>
+      <c r="G60" s="82"/>
+      <c r="H60" s="82"/>
+      <c r="I60" s="83"/>
     </row>
     <row r="61" spans="1:47" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="6"/>
@@ -7541,12 +7541,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="16">
-    <mergeCell ref="A59:I60"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:B58"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="A33:A37"/>
@@ -7557,6 +7551,12 @@
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A18:A24"/>
     <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A59:I60"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:B58"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="53" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -7571,8 +7571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO774"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="38.4" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -7586,15 +7586,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" s="1" customFormat="1" ht="369" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="99"/>
-      <c r="B1" s="100"/>
-      <c r="C1" s="79" t="s">
+      <c r="A1" s="98"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="90" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
       <c r="H1" s="32" t="s">
         <v>136</v>
       </c>
@@ -7636,19 +7636,19 @@
       <c r="AO1" s="3"/>
     </row>
     <row r="2" spans="1:41" ht="78" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="91" t="s">
         <v>198</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="91" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="84" t="s">
         <v>134</v>
       </c>
     </row>
@@ -7673,7 +7673,7 @@
       <c r="H3" s="12">
         <v>5</v>
       </c>
-      <c r="I3" s="92"/>
+      <c r="I3" s="85"/>
     </row>
     <row r="4" spans="1:41" s="9" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
@@ -7800,7 +7800,7 @@
       <c r="D8" s="57"/>
       <c r="E8" s="57"/>
       <c r="F8" s="74"/>
-      <c r="G8" s="116" t="s">
+      <c r="G8" s="77" t="s">
         <v>345</v>
       </c>
       <c r="H8" s="74"/>
@@ -7819,7 +7819,7 @@
       <c r="E9" s="57"/>
       <c r="F9" s="74"/>
       <c r="G9" s="57"/>
-      <c r="H9" s="116" t="s">
+      <c r="H9" s="77" t="s">
         <v>345</v>
       </c>
       <c r="I9" s="11">
@@ -7828,7 +7828,7 @@
       </c>
     </row>
     <row r="10" spans="1:41" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="97"/>
+      <c r="A10" s="101"/>
       <c r="B10" s="11" t="s">
         <v>204</v>
       </c>
@@ -7837,7 +7837,7 @@
       <c r="E10" s="57"/>
       <c r="F10" s="74"/>
       <c r="G10" s="57"/>
-      <c r="H10" s="116" t="s">
+      <c r="H10" s="77" t="s">
         <v>345</v>
       </c>
       <c r="I10" s="11">
@@ -7929,7 +7929,7 @@
       <c r="E15" s="57"/>
       <c r="F15" s="57"/>
       <c r="G15" s="57"/>
-      <c r="H15" s="116" t="s">
+      <c r="H15" s="77" t="s">
         <v>345</v>
       </c>
       <c r="I15" s="11">
@@ -8020,7 +8020,7 @@
       <c r="D20" s="57"/>
       <c r="E20" s="57"/>
       <c r="F20" s="57"/>
-      <c r="G20" s="116" t="s">
+      <c r="G20" s="77" t="s">
         <v>345</v>
       </c>
       <c r="H20" s="55"/>
@@ -8095,7 +8095,7 @@
       <c r="E24" s="57"/>
       <c r="F24" s="57"/>
       <c r="G24" s="57"/>
-      <c r="H24" s="116" t="s">
+      <c r="H24" s="77" t="s">
         <v>345</v>
       </c>
       <c r="I24" s="11">
@@ -8112,7 +8112,7 @@
       <c r="D25" s="57"/>
       <c r="E25" s="57"/>
       <c r="F25" s="57"/>
-      <c r="G25" s="116" t="s">
+      <c r="G25" s="77" t="s">
         <v>345</v>
       </c>
       <c r="H25" s="55"/>
@@ -8158,7 +8158,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" s="44" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="97"/>
+      <c r="A28" s="101"/>
       <c r="B28" s="11" t="s">
         <v>222</v>
       </c>
@@ -8322,13 +8322,13 @@
       </c>
     </row>
     <row r="37" spans="1:9" s="44" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="97"/>
+      <c r="A37" s="101"/>
       <c r="B37" s="11" t="s">
         <v>231</v>
       </c>
       <c r="C37" s="53"/>
       <c r="D37" s="57"/>
-      <c r="E37" s="116" t="s">
+      <c r="E37" s="77" t="s">
         <v>345</v>
       </c>
       <c r="F37" s="57"/>
@@ -8432,7 +8432,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" s="44" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="97"/>
+      <c r="A43" s="101"/>
       <c r="B43" s="11" t="s">
         <v>237</v>
       </c>
@@ -8441,7 +8441,7 @@
       <c r="E43" s="57"/>
       <c r="F43" s="57"/>
       <c r="G43" s="57"/>
-      <c r="H43" s="116" t="s">
+      <c r="H43" s="77" t="s">
         <v>345</v>
       </c>
       <c r="I43" s="11">
@@ -8542,7 +8542,7 @@
       </c>
     </row>
     <row r="49" spans="1:40" s="44" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="97"/>
+      <c r="A49" s="101"/>
       <c r="B49" s="11" t="s">
         <v>243</v>
       </c>
@@ -8659,7 +8659,7 @@
       <c r="C55" s="53"/>
       <c r="D55" s="57"/>
       <c r="E55" s="57"/>
-      <c r="F55" s="116" t="s">
+      <c r="F55" s="77" t="s">
         <v>345</v>
       </c>
       <c r="G55" s="57"/>
@@ -8684,7 +8684,7 @@
       <c r="H56" s="10"/>
       <c r="I56" s="10">
         <f>(SUM(I57:I60))/4</f>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="J56" s="44"/>
       <c r="K56" s="44"/>
@@ -8775,72 +8775,72 @@
       </c>
     </row>
     <row r="60" spans="1:40" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="97"/>
+      <c r="A60" s="101"/>
       <c r="B60" s="11" t="s">
         <v>254</v>
       </c>
       <c r="C60" s="53"/>
       <c r="D60" s="53"/>
       <c r="E60" s="53"/>
-      <c r="F60" s="53" t="s">
+      <c r="F60" s="53"/>
+      <c r="G60" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="G60" s="53"/>
       <c r="H60" s="53"/>
       <c r="I60" s="11">
         <f t="shared" si="6"/>
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:40" s="44" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="98"/>
-      <c r="B61" s="98"/>
+      <c r="A61" s="97"/>
+      <c r="B61" s="97"/>
     </row>
     <row r="62" spans="1:40" s="44" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="94" t="s">
+      <c r="A62" s="102" t="s">
         <v>255</v>
       </c>
-      <c r="B62" s="94"/>
-      <c r="C62" s="94"/>
-      <c r="D62" s="94"/>
-      <c r="E62" s="94"/>
-      <c r="F62" s="94"/>
-      <c r="G62" s="94"/>
-      <c r="H62" s="94"/>
-      <c r="I62" s="94"/>
+      <c r="B62" s="102"/>
+      <c r="C62" s="102"/>
+      <c r="D62" s="102"/>
+      <c r="E62" s="102"/>
+      <c r="F62" s="102"/>
+      <c r="G62" s="102"/>
+      <c r="H62" s="102"/>
+      <c r="I62" s="102"/>
     </row>
     <row r="63" spans="1:40" s="44" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="94"/>
-      <c r="B63" s="94"/>
-      <c r="C63" s="94"/>
-      <c r="D63" s="94"/>
-      <c r="E63" s="94"/>
-      <c r="F63" s="94"/>
-      <c r="G63" s="94"/>
-      <c r="H63" s="94"/>
-      <c r="I63" s="94"/>
+      <c r="A63" s="102"/>
+      <c r="B63" s="102"/>
+      <c r="C63" s="102"/>
+      <c r="D63" s="102"/>
+      <c r="E63" s="102"/>
+      <c r="F63" s="102"/>
+      <c r="G63" s="102"/>
+      <c r="H63" s="102"/>
+      <c r="I63" s="102"/>
     </row>
     <row r="64" spans="1:40" s="44" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="94"/>
-      <c r="B64" s="94"/>
-      <c r="C64" s="94"/>
-      <c r="D64" s="94"/>
-      <c r="E64" s="94"/>
-      <c r="F64" s="94"/>
-      <c r="G64" s="94"/>
-      <c r="H64" s="94"/>
-      <c r="I64" s="94"/>
+      <c r="A64" s="102"/>
+      <c r="B64" s="102"/>
+      <c r="C64" s="102"/>
+      <c r="D64" s="102"/>
+      <c r="E64" s="102"/>
+      <c r="F64" s="102"/>
+      <c r="G64" s="102"/>
+      <c r="H64" s="102"/>
+      <c r="I64" s="102"/>
     </row>
     <row r="65" spans="1:9" s="44" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="94"/>
-      <c r="B65" s="94"/>
-      <c r="C65" s="94"/>
-      <c r="D65" s="94"/>
-      <c r="E65" s="94"/>
-      <c r="F65" s="94"/>
-      <c r="G65" s="94"/>
-      <c r="H65" s="94"/>
-      <c r="I65" s="94"/>
+      <c r="A65" s="102"/>
+      <c r="B65" s="102"/>
+      <c r="C65" s="102"/>
+      <c r="D65" s="102"/>
+      <c r="E65" s="102"/>
+      <c r="F65" s="102"/>
+      <c r="G65" s="102"/>
+      <c r="H65" s="102"/>
+      <c r="I65" s="102"/>
     </row>
     <row r="66" spans="1:9" s="44" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="6"/>
@@ -10972,6 +10972,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ISm/sgZy1jnOXb9gvPzTBCsOht6/AMpnPlbyP7gADauIqCAZb7E9L1D7zyntouXd9W2mgl22lCvWx+szmWG0bQ==" saltValue="nO/888FW6+aUfHGWFr62Iw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="16">
+    <mergeCell ref="A62:I65"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="A30:A37"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A51:A55"/>
+    <mergeCell ref="A57:A60"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="A1:B1"/>
@@ -10981,13 +10988,6 @@
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A62:I65"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="A30:A37"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A51:A55"/>
-    <mergeCell ref="A57:A60"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="8" scale="36" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -11020,15 +11020,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" s="1" customFormat="1" ht="312.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="77"/>
-      <c r="B1" s="78"/>
-      <c r="C1" s="79" t="s">
+      <c r="A1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="90" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
       <c r="H1" s="32" t="s">
         <v>136</v>
       </c>
@@ -11072,19 +11072,19 @@
       <c r="AQ1" s="3"/>
     </row>
     <row r="2" spans="1:43" ht="78" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="91" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="84" t="s">
         <v>134</v>
       </c>
     </row>
@@ -11109,7 +11109,7 @@
       <c r="H3" s="12">
         <v>5</v>
       </c>
-      <c r="I3" s="92"/>
+      <c r="I3" s="85"/>
     </row>
     <row r="4" spans="1:43" s="9" customFormat="1" ht="62.4" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
@@ -11192,7 +11192,7 @@
       </c>
     </row>
     <row r="6" spans="1:43" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="80"/>
+      <c r="A6" s="86"/>
       <c r="B6" s="11" t="s">
         <v>23</v>
       </c>
@@ -11208,7 +11208,7 @@
       </c>
     </row>
     <row r="7" spans="1:43" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="80"/>
+      <c r="A7" s="86"/>
       <c r="B7" s="11" t="s">
         <v>24</v>
       </c>
@@ -11376,7 +11376,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" s="19" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="97"/>
+      <c r="A17" s="101"/>
       <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
@@ -11630,7 +11630,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="80">
+      <c r="A32" s="86">
         <v>7</v>
       </c>
       <c r="B32" s="11" t="s">
@@ -11648,7 +11648,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="80"/>
+      <c r="A33" s="86"/>
       <c r="B33" s="11" t="s">
         <v>44</v>
       </c>
@@ -11664,7 +11664,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="80"/>
+      <c r="A34" s="86"/>
       <c r="B34" s="11" t="s">
         <v>46</v>
       </c>
@@ -11691,28 +11691,28 @@
       <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9" s="19" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="85" t="s">
+      <c r="A36" s="78" t="s">
         <v>141</v>
       </c>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="86"/>
-      <c r="I36" s="87"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="79"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="80"/>
     </row>
     <row r="37" spans="1:9" s="19" customFormat="1" ht="148.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="88"/>
-      <c r="B37" s="89"/>
-      <c r="C37" s="89"/>
-      <c r="D37" s="89"/>
-      <c r="E37" s="89"/>
-      <c r="F37" s="89"/>
-      <c r="G37" s="89"/>
-      <c r="H37" s="89"/>
-      <c r="I37" s="90"/>
+      <c r="A37" s="81"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="83"/>
     </row>
     <row r="38" spans="1:9" s="19" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22"/>
@@ -13860,11 +13860,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="DQdV6noCoU2btdmiHoHKMMf+cIsy872IYv8dOz0g2m0970qh/6ifl2wpjsNsIxKDwVPWmA7yfDgjvOP7nyHxog==" saltValue="BZQ6kkZNgY6qlz9BaQJ+Og==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:H2"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A36:I37"/>
@@ -13873,6 +13868,11 @@
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:H2"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="8" scale="51" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -13906,15 +13906,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="312.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="77"/>
-      <c r="B1" s="78"/>
-      <c r="C1" s="79" t="s">
+      <c r="A1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="90" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
       <c r="H1" s="32" t="s">
         <v>136</v>
       </c>
@@ -13929,19 +13929,19 @@
       <c r="AW1" s="1"/>
     </row>
     <row r="2" spans="1:49" ht="78" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="91" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="91" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="84" t="s">
         <v>134</v>
       </c>
     </row>
@@ -13966,7 +13966,7 @@
       <c r="H3" s="12">
         <v>5</v>
       </c>
-      <c r="I3" s="92"/>
+      <c r="I3" s="85"/>
     </row>
     <row r="4" spans="1:49" s="9" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
@@ -14056,7 +14056,7 @@
       </c>
     </row>
     <row r="6" spans="1:49" s="20" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="80">
+      <c r="A6" s="86">
         <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -14106,7 +14106,7 @@
       <c r="AO6" s="19"/>
     </row>
     <row r="7" spans="1:49" s="20" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="80"/>
+      <c r="A7" s="86"/>
       <c r="B7" s="11" t="s">
         <v>24</v>
       </c>
@@ -14238,7 +14238,7 @@
       </c>
     </row>
     <row r="13" spans="1:49" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="97"/>
+      <c r="A13" s="101"/>
       <c r="B13" s="11" t="s">
         <v>54</v>
       </c>
@@ -14272,7 +14272,7 @@
       </c>
     </row>
     <row r="15" spans="1:49" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="80">
+      <c r="A15" s="86">
         <v>3</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -14290,7 +14290,7 @@
       </c>
     </row>
     <row r="16" spans="1:49" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="80"/>
+      <c r="A16" s="86"/>
       <c r="B16" s="11" t="s">
         <v>56</v>
       </c>
@@ -14306,7 +14306,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="80"/>
+      <c r="A17" s="86"/>
       <c r="B17" s="11" t="s">
         <v>59</v>
       </c>
@@ -14322,7 +14322,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="80"/>
+      <c r="A18" s="86"/>
       <c r="B18" s="11" t="s">
         <v>57</v>
       </c>
@@ -14338,7 +14338,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="80"/>
+      <c r="A19" s="86"/>
       <c r="B19" s="11" t="s">
         <v>58</v>
       </c>
@@ -14354,7 +14354,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="80"/>
+      <c r="A20" s="86"/>
       <c r="B20" s="11" t="s">
         <v>60</v>
       </c>
@@ -14454,7 +14454,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="97"/>
+      <c r="A26" s="101"/>
       <c r="B26" s="11" t="s">
         <v>65</v>
       </c>
@@ -14488,7 +14488,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="80">
+      <c r="A28" s="86">
         <v>5</v>
       </c>
       <c r="B28" s="11" t="s">
@@ -14506,7 +14506,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" s="3" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="80"/>
+      <c r="A29" s="86"/>
       <c r="B29" s="11" t="s">
         <v>67</v>
       </c>
@@ -14522,7 +14522,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="80"/>
+      <c r="A30" s="86"/>
       <c r="B30" s="11" t="s">
         <v>69</v>
       </c>
@@ -14538,7 +14538,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="80"/>
+      <c r="A31" s="86"/>
       <c r="B31" s="11" t="s">
         <v>70</v>
       </c>
@@ -14554,7 +14554,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="80"/>
+      <c r="A32" s="86"/>
       <c r="B32" s="11" t="s">
         <v>68</v>
       </c>
@@ -14570,7 +14570,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="80"/>
+      <c r="A33" s="86"/>
       <c r="B33" s="11" t="s">
         <v>19</v>
       </c>
@@ -14586,7 +14586,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="80"/>
+      <c r="A34" s="86"/>
       <c r="B34" s="11" t="s">
         <v>72</v>
       </c>
@@ -14620,7 +14620,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="80">
+      <c r="A36" s="86">
         <v>6</v>
       </c>
       <c r="B36" s="11" t="s">
@@ -14638,7 +14638,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="80"/>
+      <c r="A37" s="86"/>
       <c r="B37" s="11" t="s">
         <v>74</v>
       </c>
@@ -14654,7 +14654,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="80"/>
+      <c r="A38" s="86"/>
       <c r="B38" s="11" t="s">
         <v>78</v>
       </c>
@@ -14670,7 +14670,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="80"/>
+      <c r="A39" s="86"/>
       <c r="B39" s="11" t="s">
         <v>120</v>
       </c>
@@ -14686,7 +14686,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" s="3" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="80"/>
+      <c r="A40" s="86"/>
       <c r="B40" s="11" t="s">
         <v>79</v>
       </c>
@@ -14720,7 +14720,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="80">
+      <c r="A42" s="86">
         <v>7</v>
       </c>
       <c r="B42" s="11" t="s">
@@ -14738,7 +14738,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="80"/>
+      <c r="A43" s="86"/>
       <c r="B43" s="11" t="s">
         <v>125</v>
       </c>
@@ -14754,7 +14754,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="80"/>
+      <c r="A44" s="86"/>
       <c r="B44" s="11" t="s">
         <v>80</v>
       </c>
@@ -14770,7 +14770,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="80"/>
+      <c r="A45" s="86"/>
       <c r="B45" s="11" t="s">
         <v>119</v>
       </c>
@@ -14786,7 +14786,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="80"/>
+      <c r="A46" s="86"/>
       <c r="B46" s="11" t="s">
         <v>81</v>
       </c>
@@ -14820,7 +14820,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="80">
+      <c r="A48" s="86">
         <v>8</v>
       </c>
       <c r="B48" s="11" t="s">
@@ -14838,7 +14838,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="80"/>
+      <c r="A49" s="86"/>
       <c r="B49" s="23" t="s">
         <v>126</v>
       </c>
@@ -14854,7 +14854,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="80"/>
+      <c r="A50" s="86"/>
       <c r="B50" s="24" t="s">
         <v>85</v>
       </c>
@@ -14870,7 +14870,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="80"/>
+      <c r="A51" s="86"/>
       <c r="B51" s="24" t="s">
         <v>118</v>
       </c>
@@ -14886,7 +14886,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="80"/>
+      <c r="A52" s="86"/>
       <c r="B52" s="11" t="s">
         <v>86</v>
       </c>
@@ -14902,7 +14902,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="80"/>
+      <c r="A53" s="86"/>
       <c r="B53" s="11" t="s">
         <v>123</v>
       </c>
@@ -14918,7 +14918,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="80"/>
+      <c r="A54" s="86"/>
       <c r="B54" s="11" t="s">
         <v>121</v>
       </c>
@@ -14940,50 +14940,50 @@
       <c r="I55" s="17"/>
     </row>
     <row r="56" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="85" t="s">
+      <c r="A56" s="78" t="s">
         <v>141</v>
       </c>
-      <c r="B56" s="86"/>
-      <c r="C56" s="86"/>
-      <c r="D56" s="86"/>
-      <c r="E56" s="86"/>
-      <c r="F56" s="86"/>
-      <c r="G56" s="86"/>
-      <c r="H56" s="86"/>
-      <c r="I56" s="87"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="79"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="79"/>
+      <c r="F56" s="79"/>
+      <c r="G56" s="79"/>
+      <c r="H56" s="79"/>
+      <c r="I56" s="80"/>
     </row>
     <row r="57" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="102"/>
-      <c r="B57" s="103"/>
-      <c r="C57" s="103"/>
-      <c r="D57" s="103"/>
-      <c r="E57" s="103"/>
-      <c r="F57" s="103"/>
-      <c r="G57" s="103"/>
-      <c r="H57" s="103"/>
-      <c r="I57" s="104"/>
+      <c r="A57" s="103"/>
+      <c r="B57" s="104"/>
+      <c r="C57" s="104"/>
+      <c r="D57" s="104"/>
+      <c r="E57" s="104"/>
+      <c r="F57" s="104"/>
+      <c r="G57" s="104"/>
+      <c r="H57" s="104"/>
+      <c r="I57" s="105"/>
     </row>
     <row r="58" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="102"/>
-      <c r="B58" s="103"/>
-      <c r="C58" s="103"/>
-      <c r="D58" s="103"/>
-      <c r="E58" s="103"/>
-      <c r="F58" s="103"/>
-      <c r="G58" s="103"/>
-      <c r="H58" s="103"/>
-      <c r="I58" s="104"/>
+      <c r="A58" s="103"/>
+      <c r="B58" s="104"/>
+      <c r="C58" s="104"/>
+      <c r="D58" s="104"/>
+      <c r="E58" s="104"/>
+      <c r="F58" s="104"/>
+      <c r="G58" s="104"/>
+      <c r="H58" s="104"/>
+      <c r="I58" s="105"/>
     </row>
     <row r="59" spans="1:9" s="3" customFormat="1" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="88"/>
-      <c r="B59" s="89"/>
-      <c r="C59" s="89"/>
-      <c r="D59" s="89"/>
-      <c r="E59" s="89"/>
-      <c r="F59" s="89"/>
-      <c r="G59" s="89"/>
-      <c r="H59" s="89"/>
-      <c r="I59" s="90"/>
+      <c r="A59" s="81"/>
+      <c r="B59" s="82"/>
+      <c r="C59" s="82"/>
+      <c r="D59" s="82"/>
+      <c r="E59" s="82"/>
+      <c r="F59" s="82"/>
+      <c r="G59" s="82"/>
+      <c r="H59" s="82"/>
+      <c r="I59" s="83"/>
     </row>
     <row r="60" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="6"/>
@@ -17161,15 +17161,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="312.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="77"/>
-      <c r="B1" s="78"/>
-      <c r="C1" s="114" t="s">
+      <c r="A1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="115"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="107"/>
       <c r="H1" s="36" t="s">
         <v>136</v>
       </c>
@@ -17179,19 +17179,19 @@
       </c>
     </row>
     <row r="2" spans="1:45" ht="77.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="91" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="113" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="116" t="s">
         <v>134</v>
       </c>
     </row>
@@ -17216,7 +17216,7 @@
       <c r="H3" s="12">
         <v>5</v>
       </c>
-      <c r="I3" s="92"/>
+      <c r="I3" s="85"/>
     </row>
     <row r="4" spans="1:45" s="9" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
@@ -17338,7 +17338,7 @@
       </c>
     </row>
     <row r="8" spans="1:45" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="80">
+      <c r="A8" s="86">
         <v>2</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -17356,7 +17356,7 @@
       </c>
     </row>
     <row r="9" spans="1:45" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="80"/>
+      <c r="A9" s="86"/>
       <c r="B9" s="11" t="s">
         <v>92</v>
       </c>
@@ -17372,7 +17372,7 @@
       </c>
     </row>
     <row r="10" spans="1:45" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="80"/>
+      <c r="A10" s="86"/>
       <c r="B10" s="11" t="s">
         <v>90</v>
       </c>
@@ -17388,7 +17388,7 @@
       </c>
     </row>
     <row r="11" spans="1:45" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="80"/>
+      <c r="A11" s="86"/>
       <c r="B11" s="11" t="s">
         <v>95</v>
       </c>
@@ -17422,7 +17422,7 @@
       </c>
     </row>
     <row r="13" spans="1:45" s="3" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="80">
+      <c r="A13" s="86">
         <v>3</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -17440,7 +17440,7 @@
       </c>
     </row>
     <row r="14" spans="1:45" s="3" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="80"/>
+      <c r="A14" s="86"/>
       <c r="B14" s="11" t="s">
         <v>96</v>
       </c>
@@ -17456,7 +17456,7 @@
       </c>
     </row>
     <row r="15" spans="1:45" s="3" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="80"/>
+      <c r="A15" s="86"/>
       <c r="B15" s="11" t="s">
         <v>97</v>
       </c>
@@ -17672,7 +17672,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="97"/>
+      <c r="A28" s="101"/>
       <c r="B28" s="11" t="s">
         <v>131</v>
       </c>
@@ -17706,7 +17706,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" s="3" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="80">
+      <c r="A30" s="86">
         <v>6</v>
       </c>
       <c r="B30" s="11" t="s">
@@ -17724,7 +17724,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" s="3" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="80"/>
+      <c r="A31" s="86"/>
       <c r="B31" s="11" t="s">
         <v>117</v>
       </c>
@@ -17740,7 +17740,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="80"/>
+      <c r="A32" s="86"/>
       <c r="B32" s="11" t="s">
         <v>110</v>
       </c>
@@ -17756,7 +17756,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="80"/>
+      <c r="A33" s="86"/>
       <c r="B33" s="11" t="s">
         <v>20</v>
       </c>
@@ -17772,7 +17772,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="80"/>
+      <c r="A34" s="86"/>
       <c r="B34" s="11" t="s">
         <v>124</v>
       </c>
@@ -17788,7 +17788,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" s="3" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="80"/>
+      <c r="A35" s="86"/>
       <c r="B35" s="11" t="s">
         <v>127</v>
       </c>
@@ -17888,7 +17888,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="97"/>
+      <c r="A41" s="101"/>
       <c r="B41" s="11" t="s">
         <v>113</v>
       </c>
@@ -17922,7 +17922,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="80">
+      <c r="A43" s="86">
         <v>8</v>
       </c>
       <c r="B43" s="11" t="s">
@@ -17940,7 +17940,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="80"/>
+      <c r="A44" s="86"/>
       <c r="B44" s="11" t="s">
         <v>115</v>
       </c>
@@ -17956,7 +17956,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="80"/>
+      <c r="A45" s="86"/>
       <c r="B45" s="11" t="s">
         <v>116</v>
       </c>
@@ -17975,50 +17975,50 @@
       <c r="A46" s="6"/>
     </row>
     <row r="47" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="105" t="s">
+      <c r="A47" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="B47" s="93"/>
-      <c r="C47" s="93"/>
-      <c r="D47" s="93"/>
-      <c r="E47" s="93"/>
-      <c r="F47" s="93"/>
-      <c r="G47" s="93"/>
-      <c r="H47" s="93"/>
-      <c r="I47" s="106"/>
+      <c r="B47" s="87"/>
+      <c r="C47" s="87"/>
+      <c r="D47" s="87"/>
+      <c r="E47" s="87"/>
+      <c r="F47" s="87"/>
+      <c r="G47" s="87"/>
+      <c r="H47" s="87"/>
+      <c r="I47" s="109"/>
     </row>
     <row r="48" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="107"/>
-      <c r="B48" s="108"/>
-      <c r="C48" s="108"/>
-      <c r="D48" s="108"/>
-      <c r="E48" s="108"/>
-      <c r="F48" s="108"/>
-      <c r="G48" s="108"/>
-      <c r="H48" s="108"/>
-      <c r="I48" s="109"/>
+      <c r="A48" s="110"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="111"/>
+      <c r="D48" s="111"/>
+      <c r="E48" s="111"/>
+      <c r="F48" s="111"/>
+      <c r="G48" s="111"/>
+      <c r="H48" s="111"/>
+      <c r="I48" s="112"/>
     </row>
     <row r="49" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="107"/>
-      <c r="B49" s="108"/>
-      <c r="C49" s="108"/>
-      <c r="D49" s="108"/>
-      <c r="E49" s="108"/>
-      <c r="F49" s="108"/>
-      <c r="G49" s="108"/>
-      <c r="H49" s="108"/>
-      <c r="I49" s="109"/>
+      <c r="A49" s="110"/>
+      <c r="B49" s="111"/>
+      <c r="C49" s="111"/>
+      <c r="D49" s="111"/>
+      <c r="E49" s="111"/>
+      <c r="F49" s="111"/>
+      <c r="G49" s="111"/>
+      <c r="H49" s="111"/>
+      <c r="I49" s="112"/>
     </row>
     <row r="50" spans="1:9" s="3" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="110"/>
-      <c r="B50" s="111"/>
-      <c r="C50" s="111"/>
-      <c r="D50" s="111"/>
-      <c r="E50" s="111"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="111"/>
-      <c r="H50" s="111"/>
-      <c r="I50" s="112"/>
+      <c r="A50" s="113"/>
+      <c r="B50" s="114"/>
+      <c r="C50" s="114"/>
+      <c r="D50" s="114"/>
+      <c r="E50" s="114"/>
+      <c r="F50" s="114"/>
+      <c r="G50" s="114"/>
+      <c r="H50" s="114"/>
+      <c r="I50" s="115"/>
     </row>
     <row r="51" spans="1:9" s="3" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
@@ -20150,6 +20150,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="cOTlzQAOyX3CnM/Ki+QkyAzEkAjLl8ofvj2gsg4+RRT4GoPjuiqe7X8kxcTuwj9pv/61a2899Kf/AA+GAYW2zA==" saltValue="nxJUSf3HaZh9IkdUPeMGzg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="13">
+    <mergeCell ref="A47:I50"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="A30:A35"/>
@@ -20157,12 +20163,6 @@
     <mergeCell ref="A43:A45"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A22:A28"/>
-    <mergeCell ref="A47:I50"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="I2:I3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="51" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -20196,15 +20196,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="1" customFormat="1" ht="312.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="77"/>
-      <c r="B1" s="78"/>
-      <c r="C1" s="114" t="s">
+      <c r="A1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="115"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="107"/>
       <c r="H1" s="67" t="s">
         <v>136</v>
       </c>
@@ -20249,19 +20249,19 @@
       <c r="AR1" s="3"/>
     </row>
     <row r="2" spans="1:50" ht="78" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="91" t="s">
         <v>342</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="113" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="116" t="s">
         <v>134</v>
       </c>
     </row>
@@ -20286,7 +20286,7 @@
       <c r="H3" s="12">
         <v>5</v>
       </c>
-      <c r="I3" s="92"/>
+      <c r="I3" s="85"/>
     </row>
     <row r="4" spans="1:50" s="9" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
@@ -20377,7 +20377,7 @@
       </c>
     </row>
     <row r="6" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="80">
+      <c r="A6" s="86">
         <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -20395,7 +20395,7 @@
       </c>
     </row>
     <row r="7" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="80"/>
+      <c r="A7" s="86"/>
       <c r="B7" s="11" t="s">
         <v>258</v>
       </c>
@@ -20411,7 +20411,7 @@
       </c>
     </row>
     <row r="8" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="80"/>
+      <c r="A8" s="86"/>
       <c r="B8" s="11" t="s">
         <v>259</v>
       </c>
@@ -20427,7 +20427,7 @@
       </c>
     </row>
     <row r="9" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="80"/>
+      <c r="A9" s="86"/>
       <c r="B9" s="11" t="s">
         <v>294</v>
       </c>
@@ -20461,7 +20461,7 @@
       </c>
     </row>
     <row r="11" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="80">
+      <c r="A11" s="86">
         <v>2</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -20479,7 +20479,7 @@
       </c>
     </row>
     <row r="12" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="80"/>
+      <c r="A12" s="86"/>
       <c r="B12" s="61" t="s">
         <v>267</v>
       </c>
@@ -20495,7 +20495,7 @@
       </c>
     </row>
     <row r="13" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="80"/>
+      <c r="A13" s="86"/>
       <c r="B13" s="11" t="s">
         <v>269</v>
       </c>
@@ -20529,7 +20529,7 @@
       </c>
     </row>
     <row r="15" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="80">
+      <c r="A15" s="86">
         <v>3</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -20547,7 +20547,7 @@
       </c>
     </row>
     <row r="16" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="80"/>
+      <c r="A16" s="86"/>
       <c r="B16" s="11" t="s">
         <v>296</v>
       </c>
@@ -20563,7 +20563,7 @@
       </c>
     </row>
     <row r="17" spans="1:51" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="80"/>
+      <c r="A17" s="86"/>
       <c r="B17" s="11" t="s">
         <v>297</v>
       </c>
@@ -20579,7 +20579,7 @@
       </c>
     </row>
     <row r="18" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="80"/>
+      <c r="A18" s="86"/>
       <c r="B18" s="11" t="s">
         <v>298</v>
       </c>
@@ -20596,7 +20596,7 @@
       <c r="AY18" s="60"/>
     </row>
     <row r="19" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="80"/>
+      <c r="A19" s="86"/>
       <c r="B19" s="11" t="s">
         <v>299</v>
       </c>
@@ -20632,7 +20632,7 @@
       <c r="AY20" s="60"/>
     </row>
     <row r="21" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="80">
+      <c r="A21" s="86">
         <v>4</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -20651,7 +20651,7 @@
       <c r="AY21" s="60"/>
     </row>
     <row r="22" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="80"/>
+      <c r="A22" s="86"/>
       <c r="B22" s="11" t="s">
         <v>302</v>
       </c>
@@ -20668,7 +20668,7 @@
       <c r="AY22" s="60"/>
     </row>
     <row r="23" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="80"/>
+      <c r="A23" s="86"/>
       <c r="B23" s="11" t="s">
         <v>303</v>
       </c>
@@ -20685,7 +20685,7 @@
       <c r="AY23" s="60"/>
     </row>
     <row r="24" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="80"/>
+      <c r="A24" s="86"/>
       <c r="B24" s="11" t="s">
         <v>304</v>
       </c>
@@ -20702,7 +20702,7 @@
       <c r="AY24" s="60"/>
     </row>
     <row r="25" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="80"/>
+      <c r="A25" s="86"/>
       <c r="B25" s="11" t="s">
         <v>305</v>
       </c>
@@ -20738,7 +20738,7 @@
       <c r="AY26" s="60"/>
     </row>
     <row r="27" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="80">
+      <c r="A27" s="86">
         <v>5</v>
       </c>
       <c r="B27" s="11" t="s">
@@ -20757,7 +20757,7 @@
       <c r="AY27" s="60"/>
     </row>
     <row r="28" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="80"/>
+      <c r="A28" s="86"/>
       <c r="B28" s="11" t="s">
         <v>308</v>
       </c>
@@ -20774,7 +20774,7 @@
       <c r="AY28" s="60"/>
     </row>
     <row r="29" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="80"/>
+      <c r="A29" s="86"/>
       <c r="B29" s="11" t="s">
         <v>309</v>
       </c>
@@ -20810,7 +20810,7 @@
       <c r="AY30" s="60"/>
     </row>
     <row r="31" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="80">
+      <c r="A31" s="86">
         <v>6</v>
       </c>
       <c r="B31" s="11" t="s">
@@ -20829,7 +20829,7 @@
       <c r="AY31" s="60"/>
     </row>
     <row r="32" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="80"/>
+      <c r="A32" s="86"/>
       <c r="B32" s="11" t="s">
         <v>311</v>
       </c>
@@ -20846,7 +20846,7 @@
       <c r="AY32" s="60"/>
     </row>
     <row r="33" spans="1:51" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="80"/>
+      <c r="A33" s="86"/>
       <c r="B33" s="11" t="s">
         <v>312</v>
       </c>
@@ -20863,7 +20863,7 @@
       <c r="AY33" s="60"/>
     </row>
     <row r="34" spans="1:51" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="80"/>
+      <c r="A34" s="86"/>
       <c r="B34" s="11" t="s">
         <v>313</v>
       </c>
@@ -20915,7 +20915,7 @@
       </c>
     </row>
     <row r="37" spans="1:51" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="97"/>
+      <c r="A37" s="101"/>
       <c r="B37" s="11" t="s">
         <v>315</v>
       </c>
@@ -20949,7 +20949,7 @@
       </c>
     </row>
     <row r="39" spans="1:51" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="80">
+      <c r="A39" s="86">
         <v>8</v>
       </c>
       <c r="B39" s="11" t="s">
@@ -20967,7 +20967,7 @@
       </c>
     </row>
     <row r="40" spans="1:51" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="80"/>
+      <c r="A40" s="86"/>
       <c r="B40" s="11" t="s">
         <v>318</v>
       </c>
@@ -21042,7 +21042,7 @@
       <c r="AX41" s="59"/>
     </row>
     <row r="42" spans="1:51" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="80">
+      <c r="A42" s="86">
         <v>9</v>
       </c>
       <c r="B42" s="11" t="s">
@@ -21060,7 +21060,7 @@
       </c>
     </row>
     <row r="43" spans="1:51" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="80"/>
+      <c r="A43" s="86"/>
       <c r="B43" s="11" t="s">
         <v>321</v>
       </c>
@@ -28154,12 +28154,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="eWHkpZ9vOLDBOGpaMNijBUaL1v42hMNpnLLZ7QVmJIV8O0n3yUgMw0itUnkJ4kNLoCJVhI8kHmyWID/5mCjUzw==" saltValue="Rel+ZB5S70+in7sMAnLCmg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="14">
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C2:H2"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A39:A40"/>
@@ -28168,6 +28162,12 @@
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A15:A19"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C2:H2"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" scale="33" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -28201,15 +28201,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="1" customFormat="1" ht="312.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="77"/>
-      <c r="B1" s="78"/>
-      <c r="C1" s="114" t="s">
+      <c r="A1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="115"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="107"/>
       <c r="H1" s="65" t="s">
         <v>136</v>
       </c>
@@ -28254,19 +28254,19 @@
       <c r="AR1" s="3"/>
     </row>
     <row r="2" spans="1:50" ht="78" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="91" t="s">
         <v>343</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="113" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="116" t="s">
         <v>134</v>
       </c>
     </row>
@@ -28291,7 +28291,7 @@
       <c r="H3" s="12">
         <v>5</v>
       </c>
-      <c r="I3" s="92"/>
+      <c r="I3" s="85"/>
     </row>
     <row r="4" spans="1:50" s="9" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
@@ -28496,7 +28496,7 @@
       </c>
     </row>
     <row r="13" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="97"/>
+      <c r="A13" s="101"/>
       <c r="B13" s="11" t="s">
         <v>264</v>
       </c>
@@ -28530,7 +28530,7 @@
       </c>
     </row>
     <row r="15" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="80">
+      <c r="A15" s="86">
         <v>2</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -28548,7 +28548,7 @@
       </c>
     </row>
     <row r="16" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="80"/>
+      <c r="A16" s="86"/>
       <c r="B16" s="61" t="s">
         <v>267</v>
       </c>
@@ -28564,7 +28564,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="80"/>
+      <c r="A17" s="86"/>
       <c r="B17" s="61" t="s">
         <v>268</v>
       </c>
@@ -28580,7 +28580,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="80"/>
+      <c r="A18" s="86"/>
       <c r="B18" s="11" t="s">
         <v>269</v>
       </c>
@@ -28614,7 +28614,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="80">
+      <c r="A20" s="86">
         <v>3</v>
       </c>
       <c r="B20" s="11" t="s">
@@ -28632,7 +28632,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="80"/>
+      <c r="A21" s="86"/>
       <c r="B21" s="11" t="s">
         <v>272</v>
       </c>
@@ -28648,7 +28648,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="80"/>
+      <c r="A22" s="86"/>
       <c r="B22" s="11" t="s">
         <v>273</v>
       </c>
@@ -28682,7 +28682,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="80">
+      <c r="A24" s="86">
         <v>4</v>
       </c>
       <c r="B24" s="11" t="s">
@@ -28700,7 +28700,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="80"/>
+      <c r="A25" s="86"/>
       <c r="B25" s="11" t="s">
         <v>276</v>
       </c>
@@ -28716,7 +28716,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="80"/>
+      <c r="A26" s="86"/>
       <c r="B26" s="11" t="s">
         <v>277</v>
       </c>
@@ -28784,7 +28784,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="97"/>
+      <c r="A30" s="101"/>
       <c r="B30" s="11" t="s">
         <v>281</v>
       </c>
@@ -28818,7 +28818,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="80">
+      <c r="A32" s="86">
         <v>6</v>
       </c>
       <c r="B32" s="11" t="s">
@@ -28836,7 +28836,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="80"/>
+      <c r="A33" s="86"/>
       <c r="B33" s="11" t="s">
         <v>284</v>
       </c>
@@ -28852,7 +28852,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="80"/>
+      <c r="A34" s="86"/>
       <c r="B34" s="11" t="s">
         <v>285</v>
       </c>
@@ -28936,7 +28936,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="97"/>
+      <c r="A39" s="101"/>
       <c r="B39" s="11" t="s">
         <v>290</v>
       </c>
@@ -29004,7 +29004,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="97"/>
+      <c r="A43" s="101"/>
       <c r="B43" s="11" t="s">
         <v>293</v>
       </c>
@@ -36108,11 +36108,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Fx+jl4uIgM5VUcG4Q/VPa6BT1fBLoCQP0KER4PEirDq3QZzyU9iEWclN17y9UaBuO6sXhZzp6YfR4XqYu9e7Jw==" saltValue="6f0q3VNkRPAst8jLulPYNw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="13">
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A36:A39"/>
     <mergeCell ref="A41:A43"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -36121,6 +36116,11 @@
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="C1:G1"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A36:A39"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" scale="33" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -36155,15 +36155,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="1" customFormat="1" ht="312.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="77"/>
-      <c r="B1" s="78"/>
-      <c r="C1" s="114" t="s">
+      <c r="A1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="115"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="107"/>
       <c r="H1" s="36" t="s">
         <v>136</v>
       </c>
@@ -36207,19 +36207,19 @@
       <c r="AQ1" s="3"/>
     </row>
     <row r="2" spans="1:50" ht="78" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="91" t="s">
         <v>344</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="113" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="116" t="s">
         <v>134</v>
       </c>
     </row>
@@ -36244,7 +36244,7 @@
       <c r="H3" s="12">
         <v>5</v>
       </c>
-      <c r="I3" s="92"/>
+      <c r="I3" s="85"/>
     </row>
     <row r="4" spans="1:50" s="9" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
@@ -36335,7 +36335,7 @@
       </c>
     </row>
     <row r="6" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="80">
+      <c r="A6" s="86">
         <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -36353,7 +36353,7 @@
       </c>
     </row>
     <row r="7" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="80"/>
+      <c r="A7" s="86"/>
       <c r="B7" s="11" t="s">
         <v>258</v>
       </c>
@@ -36369,7 +36369,7 @@
       </c>
     </row>
     <row r="8" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="80"/>
+      <c r="A8" s="86"/>
       <c r="B8" s="11" t="s">
         <v>259</v>
       </c>
@@ -36385,7 +36385,7 @@
       </c>
     </row>
     <row r="9" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="80"/>
+      <c r="A9" s="86"/>
       <c r="B9" s="11" t="s">
         <v>294</v>
       </c>
@@ -36419,7 +36419,7 @@
       </c>
     </row>
     <row r="11" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="80">
+      <c r="A11" s="86">
         <v>2</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -36437,7 +36437,7 @@
       </c>
     </row>
     <row r="12" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="80"/>
+      <c r="A12" s="86"/>
       <c r="B12" s="61" t="s">
         <v>267</v>
       </c>
@@ -36453,7 +36453,7 @@
       </c>
     </row>
     <row r="13" spans="1:50" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="80"/>
+      <c r="A13" s="86"/>
       <c r="B13" s="11" t="s">
         <v>269</v>
       </c>
@@ -36553,7 +36553,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="97"/>
+      <c r="A19" s="101"/>
       <c r="B19" s="11" t="s">
         <v>326</v>
       </c>
@@ -36587,7 +36587,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="80">
+      <c r="A21" s="86">
         <v>4</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -36605,7 +36605,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="59" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="80"/>
+      <c r="A22" s="86"/>
       <c r="B22" s="11" t="s">
         <v>329</v>
       </c>
@@ -36639,7 +36639,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="80">
+      <c r="A24" s="86">
         <v>5</v>
       </c>
       <c r="B24" s="11" t="s">
@@ -36657,7 +36657,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="80"/>
+      <c r="A25" s="86"/>
       <c r="B25" s="11" t="s">
         <v>332</v>
       </c>
@@ -36757,7 +36757,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="97"/>
+      <c r="A31" s="101"/>
       <c r="B31" s="11" t="s">
         <v>338</v>
       </c>
@@ -36809,7 +36809,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="97"/>
+      <c r="A34" s="101"/>
       <c r="B34" s="11" t="s">
         <v>288</v>
       </c>
@@ -36843,7 +36843,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="80">
+      <c r="A36" s="86">
         <v>8</v>
       </c>
       <c r="B36" s="11" t="s">
@@ -36861,7 +36861,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" s="59" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="80"/>
+      <c r="A37" s="86"/>
       <c r="B37" s="11" t="s">
         <v>293</v>
       </c>
@@ -39679,11 +39679,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="GbA6DBXlQwqgRXCem2SDxJAdNdoDeGFJO8dbZGkvIrCKtECChgsYDSgewd2x8qUDzhmYUgrAJqL03azAQKWPvA==" saltValue="XFuPvrBaSwO1W/WgYGszbg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="13">
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A33:A34"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -39692,6 +39687,11 @@
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="C1:G1"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A33:A34"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="33" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>